<commit_message>
successfully opening device data workbook
</commit_message>
<xml_diff>
--- a/test/device/data/deviceData.xlsx
+++ b/test/device/data/deviceData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernardbussy/go/src/gitlab.com/iotTracker/brain/test/system/device/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernardbussy/go/src/gitlab.com/iotTracker/brain/test/device/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A0D32D-74BA-314E-8564-5C8348F07DC8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830252DC-4FA4-EE44-A2CE-CF2AFC1EBB27}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B8EBAA13-D693-2346-B1AA-7795BD176E59}"/>
   </bookViews>
@@ -385,7 +385,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
demo devices in work book
</commit_message>
<xml_diff>
--- a/test/device/data/deviceData.xlsx
+++ b/test/device/data/deviceData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernardbussy/go/src/gitlab.com/iotTracker/brain/test/device/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4049FA17-F54E-654B-A871-D083C4AB5217}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61F9BD6-3CF7-8C45-B43E-50DBA1E05AC0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B8EBAA13-D693-2346-B1AA-7795BD176E59}"/>
   </bookViews>
   <sheets>
-    <sheet name="DevicesToCreate" sheetId="1" r:id="rId1"/>
+    <sheet name="TK102Devices" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>TK102</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="59">
   <si>
     <t>ManufacturerId</t>
   </si>
@@ -52,13 +46,169 @@
   </si>
   <si>
     <t>AssignedId</t>
+  </si>
+  <si>
+    <t>+27</t>
+  </si>
+  <si>
+    <t>0720499352</t>
+  </si>
+  <si>
+    <t>Entity Fields</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Owner Admin Email</t>
+  </si>
+  <si>
+    <t>Assigned Admin Email</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>27045053055</t>
+  </si>
+  <si>
+    <t>27045052198</t>
+  </si>
+  <si>
+    <t>0663361197</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>27045052610</t>
+  </si>
+  <si>
+    <t>0826458429</t>
+  </si>
+  <si>
+    <t>monteagleAdmin@monteagle.com</t>
+  </si>
+  <si>
+    <t>dhlAdmin@dhl.com</t>
+  </si>
+  <si>
+    <t>picknpayAdmin@picknpay.com</t>
+  </si>
+  <si>
+    <t>reinhardAdmin@reinhard.com</t>
+  </si>
+  <si>
+    <t>sparAdmin@spar.com</t>
+  </si>
+  <si>
+    <t>83752716547</t>
+  </si>
+  <si>
+    <t>56532987613</t>
+  </si>
+  <si>
+    <t>12387645389</t>
+  </si>
+  <si>
+    <t>08436297809</t>
+  </si>
+  <si>
+    <t>12064835263</t>
+  </si>
+  <si>
+    <t>08342295636</t>
+  </si>
+  <si>
+    <t>12395673825</t>
+  </si>
+  <si>
+    <t>08645372928</t>
+  </si>
+  <si>
+    <t>98648352637</t>
+  </si>
+  <si>
+    <t>65746357265</t>
+  </si>
+  <si>
+    <t>64537207487</t>
+  </si>
+  <si>
+    <t>06374892983</t>
+  </si>
+  <si>
+    <t>83739234628</t>
+  </si>
+  <si>
+    <t>12348967363</t>
+  </si>
+  <si>
+    <t>86574839648</t>
+  </si>
+  <si>
+    <t>0675556434</t>
+  </si>
+  <si>
+    <t>0825654334</t>
+  </si>
+  <si>
+    <t>0546227456</t>
+  </si>
+  <si>
+    <t>0234557256</t>
+  </si>
+  <si>
+    <t>0564783425</t>
+  </si>
+  <si>
+    <t>0967453624</t>
+  </si>
+  <si>
+    <t>0714352678</t>
+  </si>
+  <si>
+    <t>0754635242</t>
+  </si>
+  <si>
+    <t>0828684114</t>
+  </si>
+  <si>
+    <t>0654637876</t>
+  </si>
+  <si>
+    <t>0546372554</t>
+  </si>
+  <si>
+    <t>0569987665</t>
+  </si>
+  <si>
+    <t>0113485764</t>
+  </si>
+  <si>
+    <t>0756473826</t>
+  </si>
+  <si>
+    <t>0657463527</t>
+  </si>
+  <si>
+    <t>woolworthsAdmin@woolworths.com</t>
+  </si>
+  <si>
+    <t>makroAdmin@makro.com</t>
+  </si>
+  <si>
+    <t>fruitnvegAdmin@fruitnveg.com</t>
+  </si>
+  <si>
+    <t>gameAdmin@game.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -66,16 +216,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -83,14 +255,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,52 +644,499 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68A7BEA-7AA6-554E-9902-9D1AFE01DEE8}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="13.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="4"/>
+    <col min="7" max="7" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="5"/>
+    <col min="9" max="9" width="30.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" s="7" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="E3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="I4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{DB83EC30-CC8B-C648-9BBF-A55B9FFF4BF5}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{A540EF33-B00C-C749-B210-9B8E779D683C}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{FB7C148E-D741-5849-97FB-065CE2259183}"/>
+    <hyperlink ref="J4" r:id="rId4" xr:uid="{5F0760D1-B9BE-084B-9A6E-7DCD8AF00E18}"/>
+    <hyperlink ref="I5" r:id="rId5" xr:uid="{B0A5D7EC-CED6-864F-A0BA-1DE2A866A1D4}"/>
+    <hyperlink ref="J5" r:id="rId6" xr:uid="{C5EB6FA0-997B-0341-81D3-0FD7E45B15DD}"/>
+    <hyperlink ref="J6" r:id="rId7" xr:uid="{747A78B8-E27A-D547-A3D0-9A48EC96AC55}"/>
+    <hyperlink ref="J13" r:id="rId8" xr:uid="{FCF0B47C-578C-0245-A32C-D49470AFF0F8}"/>
+    <hyperlink ref="J8" r:id="rId9" xr:uid="{3BFF9FF9-7EFB-D244-9D03-A5E3AF2BAF59}"/>
+    <hyperlink ref="J12" r:id="rId10" xr:uid="{16203D3C-2BE5-DF46-8FFF-24696364A08E}"/>
+    <hyperlink ref="J18" r:id="rId11" xr:uid="{57715E97-B986-6749-95B9-1A816BDB8789}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B3:D3 C4:D4 B4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
excel maniplulation wrappers started
</commit_message>
<xml_diff>
--- a/test/device/data/deviceData.xlsx
+++ b/test/device/data/deviceData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernardbussy/go/src/gitlab.com/iotTracker/brain/test/device/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61F9BD6-3CF7-8C45-B43E-50DBA1E05AC0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94084704-E519-1941-9CCE-A1FED6BA56F3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B8EBAA13-D693-2346-B1AA-7795BD176E59}"/>
   </bookViews>
@@ -312,12 +312,6 @@
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -329,6 +323,12 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -647,183 +647,183 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="13.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="4"/>
-    <col min="7" max="7" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="3"/>
     <col min="9" max="9" width="30.5" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" s="7" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:10" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="14" t="s">
+      <c r="E3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="14" t="s">
+      <c r="E4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="14" t="s">
+      <c r="E5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -831,42 +831,42 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="E8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="E9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -874,19 +874,19 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="4" t="s">
+      <c r="E10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -897,19 +897,19 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="4" t="s">
+      <c r="E11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -917,65 +917,65 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="4" t="s">
+      <c r="E12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="4" t="s">
+      <c r="E13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="4" t="s">
+      <c r="E14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -986,19 +986,19 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="4" t="s">
+      <c r="E15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -1006,19 +1006,19 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="4" t="s">
+      <c r="E16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -1029,19 +1029,19 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="4" t="s">
+      <c r="E17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -1052,42 +1052,42 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="4" t="s">
+      <c r="E18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="4" t="s">
+      <c r="E19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -1095,19 +1095,19 @@
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="4" t="s">
+      <c r="E20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I20" s="1" t="s">

</xml_diff>

<commit_message>
adaptor for retrieve party added
</commit_message>
<xml_diff>
--- a/test/device/data/deviceData.xlsx
+++ b/test/device/data/deviceData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernardbussy/go/src/gitlab.com/iotTracker/brain/test/device/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94084704-E519-1941-9CCE-A1FED6BA56F3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23D9034-80CD-8C4E-B021-16E33E4DCECE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B8EBAA13-D693-2346-B1AA-7795BD176E59}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="59">
   <si>
     <t>ManufacturerId</t>
   </si>
@@ -647,7 +647,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -823,9 +823,6 @@
       <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="I7" s="1" t="s">
         <v>23</v>
       </c>
@@ -866,9 +863,6 @@
       <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="I9" s="1" t="s">
         <v>23</v>
       </c>
@@ -909,9 +903,6 @@
       <c r="E11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="I11" s="1" t="s">
         <v>23</v>
       </c>
@@ -998,9 +989,6 @@
       <c r="E15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="I15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1086,9 +1074,6 @@
       </c>
       <c r="E19" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
offsets in SheetAsSliceMap fixed
</commit_message>
<xml_diff>
--- a/test/device/data/deviceData.xlsx
+++ b/test/device/data/deviceData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernardbussy/go/src/gitlab.com/iotTracker/brain/test/device/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23D9034-80CD-8C4E-B021-16E33E4DCECE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF07095-DBEE-4645-829E-2B482E06B824}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B8EBAA13-D693-2346-B1AA-7795BD176E59}"/>
   </bookViews>
@@ -647,7 +647,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
device population ready for creation working
</commit_message>
<xml_diff>
--- a/test/device/data/deviceData.xlsx
+++ b/test/device/data/deviceData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernardbussy/go/src/gitlab.com/iotTracker/brain/test/device/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1E337B-C07F-A341-99DB-7677A280753E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0691377-F5C8-E642-B8BB-B30AD254B230}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B8EBAA13-D693-2346-B1AA-7795BD176E59}"/>
   </bookViews>
@@ -647,7 +647,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -881,7 +881,7 @@
         <v>10</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>21</v>
@@ -967,7 +967,7 @@
         <v>10</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>23</v>
@@ -1007,7 +1007,7 @@
         <v>10</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>20</v>
@@ -1030,7 +1030,7 @@
         <v>10</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>21</v>
@@ -1093,7 +1093,7 @@
         <v>10</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
tk102 device administrator create added
</commit_message>
<xml_diff>
--- a/test/device/data/deviceData.xlsx
+++ b/test/device/data/deviceData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernardbussy/go/src/gitlab.com/iotTracker/brain/test/device/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0691377-F5C8-E642-B8BB-B30AD254B230}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B69452-CF44-E041-85C6-8C9FB611D053}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B8EBAA13-D693-2346-B1AA-7795BD176E59}"/>
   </bookViews>
@@ -647,7 +647,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>